<commit_message>
Updated Example to Include Result Images and .mat results
</commit_message>
<xml_diff>
--- a/Example 2D Structure/Results/Landmarks/femur_landmarks_Morph.xlsx
+++ b/Example 2D Structure/Results/Landmarks/femur_landmarks_Morph.xlsx
@@ -13,7 +13,112 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+  <si>
+    <t>Landmark</t>
+  </si>
+  <si>
+    <t>ACL_AM1</t>
+  </si>
+  <si>
+    <t>ACL_AM2</t>
+  </si>
+  <si>
+    <t>ACL_PL1</t>
+  </si>
+  <si>
+    <t>ACL_PL2</t>
+  </si>
+  <si>
+    <t>PCL_AL1</t>
+  </si>
+  <si>
+    <t>PCL_AL2</t>
+  </si>
+  <si>
+    <t>PCL_PM1</t>
+  </si>
+  <si>
+    <t>PCL_PM2</t>
+  </si>
+  <si>
+    <t>LCL_1</t>
+  </si>
+  <si>
+    <t>LCL_2</t>
+  </si>
+  <si>
+    <t>LCL_3</t>
+  </si>
+  <si>
+    <t>MCL_Ant</t>
+  </si>
+  <si>
+    <t>MCL_Med</t>
+  </si>
+  <si>
+    <t>MCL_Post</t>
+  </si>
+  <si>
+    <t>MCL_D1</t>
+  </si>
+  <si>
+    <t>MCL_D2</t>
+  </si>
+  <si>
+    <t>MCL_D3</t>
+  </si>
+  <si>
+    <t>ALS_1</t>
+  </si>
+  <si>
+    <t>ALS_2</t>
+  </si>
+  <si>
+    <t>ALS_3</t>
+  </si>
+  <si>
+    <t>PFL_1</t>
+  </si>
+  <si>
+    <t>PFL_2</t>
+  </si>
+  <si>
+    <t>PFL_3</t>
+  </si>
+  <si>
+    <t>POL_1</t>
+  </si>
+  <si>
+    <t>POL_2</t>
+  </si>
+  <si>
+    <t>PCAPL_1</t>
+  </si>
+  <si>
+    <t>PCAPL_2</t>
+  </si>
+  <si>
+    <t>PCAPL_3</t>
+  </si>
+  <si>
+    <t>PCAPM_1</t>
+  </si>
+  <si>
+    <t>PCAPM_2</t>
+  </si>
+  <si>
+    <t>PCAPM_3</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
   <si>
     <t>Landmark</t>
   </si>
@@ -174,21 +279,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="B2" s="0">
         <v>2.2744272057041837</v>
@@ -202,7 +307,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B3" s="0">
         <v>2.4045878209497982</v>
@@ -216,7 +321,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="B4" s="0">
         <v>4.6537046418728032</v>
@@ -230,7 +335,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B5" s="0">
         <v>2.1842620102543564</v>
@@ -244,7 +349,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B6" s="0">
         <v>-10.76150538204115</v>
@@ -258,7 +363,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="B7" s="0">
         <v>-11.213078019923255</v>
@@ -272,7 +377,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="B8" s="0">
         <v>-12.512963309568962</v>
@@ -286,7 +391,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B9" s="0">
         <v>-12.656563676062703</v>
@@ -300,7 +405,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0">
         <v>40.42691839772133</v>
@@ -314,7 +419,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="B11" s="0">
         <v>40.298115397432582</v>
@@ -328,7 +433,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B12" s="0">
         <v>38.490982653149501</v>
@@ -342,7 +447,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B13" s="0">
         <v>-43.655600851358791</v>
@@ -356,7 +461,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="B14" s="0">
         <v>-42.581335615294613</v>
@@ -370,7 +475,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="B15" s="0">
         <v>-39.766692158703506</v>
@@ -384,7 +489,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="B16" s="0">
         <v>-45.028376068461434</v>
@@ -398,7 +503,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="B17" s="0">
         <v>-42.054889404277887</v>
@@ -412,7 +517,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B18" s="0">
         <v>-39.099878902598675</v>
@@ -426,7 +531,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B19" s="0">
         <v>41.20920393234006</v>
@@ -440,7 +545,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="B20" s="0">
         <v>40.831051919097604</v>
@@ -454,7 +559,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B21" s="0">
         <v>40.756127763577439</v>
@@ -468,7 +573,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B22" s="0">
         <v>37.110571473229832</v>
@@ -482,7 +587,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B23" s="0">
         <v>38.393297810671541</v>
@@ -496,7 +601,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B24" s="0">
         <v>38.253100393819551</v>
@@ -510,7 +615,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="B25" s="0">
         <v>-40.318467111019302</v>
@@ -524,7 +629,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="B26" s="0">
         <v>-38.984214045894035</v>
@@ -538,7 +643,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B27" s="0">
         <v>28.811557578242127</v>
@@ -552,7 +657,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B28" s="0">
         <v>17.723057348900163</v>
@@ -566,7 +671,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="B29" s="0">
         <v>9.9105013240325057</v>
@@ -580,7 +685,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="B30" s="0">
         <v>-11.488892111621679</v>
@@ -594,7 +699,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B31" s="0">
         <v>-21.322593585811823</v>
@@ -608,7 +713,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="B32" s="0">
         <v>-36.241266523300048</v>

</xml_diff>

<commit_message>
Added Polyak Momentum Term and Updated Figure Results
</commit_message>
<xml_diff>
--- a/Example 2D Structure/Results/Landmarks/femur_landmarks_Morph.xlsx
+++ b/Example 2D Structure/Results/Landmarks/femur_landmarks_Morph.xlsx
@@ -13,7 +13,112 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+  <si>
+    <t>Landmark</t>
+  </si>
+  <si>
+    <t>ACL_AM1</t>
+  </si>
+  <si>
+    <t>ACL_AM2</t>
+  </si>
+  <si>
+    <t>ACL_PL1</t>
+  </si>
+  <si>
+    <t>ACL_PL2</t>
+  </si>
+  <si>
+    <t>PCL_AL1</t>
+  </si>
+  <si>
+    <t>PCL_AL2</t>
+  </si>
+  <si>
+    <t>PCL_PM1</t>
+  </si>
+  <si>
+    <t>PCL_PM2</t>
+  </si>
+  <si>
+    <t>LCL_1</t>
+  </si>
+  <si>
+    <t>LCL_2</t>
+  </si>
+  <si>
+    <t>LCL_3</t>
+  </si>
+  <si>
+    <t>MCL_Ant</t>
+  </si>
+  <si>
+    <t>MCL_Med</t>
+  </si>
+  <si>
+    <t>MCL_Post</t>
+  </si>
+  <si>
+    <t>MCL_D1</t>
+  </si>
+  <si>
+    <t>MCL_D2</t>
+  </si>
+  <si>
+    <t>MCL_D3</t>
+  </si>
+  <si>
+    <t>ALS_1</t>
+  </si>
+  <si>
+    <t>ALS_2</t>
+  </si>
+  <si>
+    <t>ALS_3</t>
+  </si>
+  <si>
+    <t>PFL_1</t>
+  </si>
+  <si>
+    <t>PFL_2</t>
+  </si>
+  <si>
+    <t>PFL_3</t>
+  </si>
+  <si>
+    <t>POL_1</t>
+  </si>
+  <si>
+    <t>POL_2</t>
+  </si>
+  <si>
+    <t>PCAPL_1</t>
+  </si>
+  <si>
+    <t>PCAPL_2</t>
+  </si>
+  <si>
+    <t>PCAPL_3</t>
+  </si>
+  <si>
+    <t>PCAPM_1</t>
+  </si>
+  <si>
+    <t>PCAPM_2</t>
+  </si>
+  <si>
+    <t>PCAPM_3</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
   <si>
     <t>Landmark</t>
   </si>
@@ -271,458 +376,458 @@
   <dimension ref="A1:D32"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.48828125" customWidth="true"/>
-    <col min="2" max="2" width="12.37890625" customWidth="true"/>
+    <col min="1" max="1" width="9.85546875" customWidth="true"/>
+    <col min="2" max="2" width="12.42578125" customWidth="true"/>
     <col min="3" max="3" width="11.7109375" customWidth="true"/>
     <col min="4" max="4" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="B2" s="0">
-        <v>2.2744272057041837</v>
+        <v>2.2483823375766208</v>
       </c>
       <c r="C2" s="0">
-        <v>17.959607826115306</v>
+        <v>18.011546205610252</v>
       </c>
       <c r="D2" s="0">
-        <v>15.092281158446314</v>
+        <v>15.086522852935371</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="B3" s="0">
-        <v>2.4045878209497982</v>
+        <v>2.4107639775420577</v>
       </c>
       <c r="C3" s="0">
-        <v>20.268636461193516</v>
+        <v>20.369763188336471</v>
       </c>
       <c r="D3" s="0">
-        <v>14.087710413140465</v>
+        <v>14.100090737896041</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="B4" s="0">
-        <v>4.6537046418728032</v>
+        <v>4.6600184659661625</v>
       </c>
       <c r="C4" s="0">
-        <v>16.958451112874918</v>
+        <v>16.941927990659938</v>
       </c>
       <c r="D4" s="0">
-        <v>8.687754159383811</v>
+        <v>8.7180985036830307</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B5" s="0">
-        <v>2.1842620102543564</v>
+        <v>2.168594022029243</v>
       </c>
       <c r="C5" s="0">
-        <v>17.304473810672842</v>
+        <v>17.319803417587377</v>
       </c>
       <c r="D5" s="0">
-        <v>10.640558399903945</v>
+        <v>10.661397614943111</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="B6" s="0">
-        <v>-10.76150538204115</v>
+        <v>-10.6782445138626</v>
       </c>
       <c r="C6" s="0">
-        <v>16.509607532482136</v>
+        <v>16.52524269391866</v>
       </c>
       <c r="D6" s="0">
-        <v>12.688432589536616</v>
+        <v>12.544157943275824</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="B7" s="0">
-        <v>-11.213078019923255</v>
+        <v>-11.123440988617357</v>
       </c>
       <c r="C7" s="0">
-        <v>16.671240540754521</v>
+        <v>16.653526688921886</v>
       </c>
       <c r="D7" s="0">
-        <v>9.2555829854832101</v>
+        <v>9.1575794368873034</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="B8" s="0">
-        <v>-12.512963309568962</v>
+        <v>-12.417738656417121</v>
       </c>
       <c r="C8" s="0">
-        <v>17.986766362966055</v>
+        <v>17.993513417248838</v>
       </c>
       <c r="D8" s="0">
-        <v>11.662552904573845</v>
+        <v>11.516940843786514</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="B9" s="0">
-        <v>-12.656563676062703</v>
+        <v>-12.571327297883769</v>
       </c>
       <c r="C9" s="0">
-        <v>18.762360704574053</v>
+        <v>18.755564073126521</v>
       </c>
       <c r="D9" s="0">
-        <v>8.7946539793956848</v>
+        <v>8.7075450391447298</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="B10" s="0">
-        <v>40.42691839772133</v>
+        <v>40.315200017356041</v>
       </c>
       <c r="C10" s="0">
-        <v>10.938008076846383</v>
+        <v>11.14103554976106</v>
       </c>
       <c r="D10" s="0">
-        <v>8.9872262826020872</v>
+        <v>8.7217749276246828</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B11" s="0">
-        <v>40.298115397432582</v>
+        <v>40.195438623577346</v>
       </c>
       <c r="C11" s="0">
-        <v>13.430893234453915</v>
+        <v>13.644098858355024</v>
       </c>
       <c r="D11" s="0">
-        <v>9.325678473513916</v>
+        <v>9.0868152619816929</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="B12" s="0">
-        <v>38.490982653149501</v>
+        <v>38.386142761120276</v>
       </c>
       <c r="C12" s="0">
-        <v>14.701686196289183</v>
+        <v>14.947572152086259</v>
       </c>
       <c r="D12" s="0">
-        <v>9.5534140116728796</v>
+        <v>9.3252087193500657</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="B13" s="0">
-        <v>-43.655600851358791</v>
+        <v>-43.711614242018548</v>
       </c>
       <c r="C13" s="0">
-        <v>4.1902697322839018</v>
+        <v>4.4660043246097985</v>
       </c>
       <c r="D13" s="0">
-        <v>20.820198783505528</v>
+        <v>20.688447645834287</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="B14" s="0">
-        <v>-42.581335615294613</v>
+        <v>-42.671362445426794</v>
       </c>
       <c r="C14" s="0">
-        <v>11.504634516102149</v>
+        <v>11.613376667260885</v>
       </c>
       <c r="D14" s="0">
-        <v>20.235896757070453</v>
+        <v>19.977697258530807</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="B15" s="0">
-        <v>-39.766692158703506</v>
+        <v>-39.831366223563968</v>
       </c>
       <c r="C15" s="0">
-        <v>18.510196708501301</v>
+        <v>18.454591628516582</v>
       </c>
       <c r="D15" s="0">
-        <v>19.2354770643244</v>
+        <v>19.085111823550118</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="B16" s="0">
-        <v>-45.028376068461434</v>
+        <v>-45.053217382054697</v>
       </c>
       <c r="C16" s="0">
-        <v>7.745876537708213</v>
+        <v>7.82536437087533</v>
       </c>
       <c r="D16" s="0">
-        <v>12.564143274240639</v>
+        <v>12.538433704522019</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="B17" s="0">
-        <v>-42.054889404277887</v>
+        <v>-42.082459482324161</v>
       </c>
       <c r="C17" s="0">
-        <v>12.572115483334773</v>
+        <v>12.579215181039181</v>
       </c>
       <c r="D17" s="0">
-        <v>11.286368741742153</v>
+        <v>11.254700802962256</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="B18" s="0">
-        <v>-39.099878902598675</v>
+        <v>-39.108122090382764</v>
       </c>
       <c r="C18" s="0">
-        <v>17.224407548072445</v>
+        <v>17.206336369660452</v>
       </c>
       <c r="D18" s="0">
-        <v>10.316430418425798</v>
+        <v>10.314825999972834</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="B19" s="0">
-        <v>41.20920393234006</v>
+        <v>41.127390106883986</v>
       </c>
       <c r="C19" s="0">
-        <v>5.0229038836795574</v>
+        <v>5.0844281756616523</v>
       </c>
       <c r="D19" s="0">
-        <v>11.370218688108853</v>
+        <v>11.226907085891133</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="B20" s="0">
-        <v>40.831051919097604</v>
+        <v>40.726429801347308</v>
       </c>
       <c r="C20" s="0">
-        <v>7.9294359465916404</v>
+        <v>8.0786209193035887</v>
       </c>
       <c r="D20" s="0">
-        <v>10.238336128975561</v>
+        <v>9.9982325507097194</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="B21" s="0">
-        <v>40.756127763577439</v>
+        <v>40.648067595255206</v>
       </c>
       <c r="C21" s="0">
-        <v>10.661654740530585</v>
+        <v>10.859303029494653</v>
       </c>
       <c r="D21" s="0">
-        <v>9.8714990208170175</v>
+        <v>9.6126989259103031</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B22" s="0">
-        <v>37.110571473229832</v>
+        <v>36.977710520601562</v>
       </c>
       <c r="C22" s="0">
-        <v>14.351425217775061</v>
+        <v>14.765515469111204</v>
       </c>
       <c r="D22" s="0">
-        <v>5.9132235692534056</v>
+        <v>5.6275658245338116</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="B23" s="0">
-        <v>38.393297810671541</v>
+        <v>38.313921786951475</v>
       </c>
       <c r="C23" s="0">
-        <v>18.309828992745402</v>
+        <v>18.724344100627842</v>
       </c>
       <c r="D23" s="0">
-        <v>6.9250971455621286</v>
+        <v>6.7624971952186792</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="B24" s="0">
-        <v>38.253100393819551</v>
+        <v>38.17880435243746</v>
       </c>
       <c r="C24" s="0">
-        <v>21.187898717978552</v>
+        <v>21.511474965780028</v>
       </c>
       <c r="D24" s="0">
-        <v>7.9225293793815004</v>
+        <v>7.8175632382706386</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="B25" s="0">
-        <v>-40.318467111019302</v>
+        <v>-40.302667457108271</v>
       </c>
       <c r="C25" s="0">
-        <v>14.536601839756193</v>
+        <v>14.520728471293964</v>
       </c>
       <c r="D25" s="0">
-        <v>6.9850288060362411</v>
+        <v>7.0154751073601203</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B26" s="0">
-        <v>-38.984214045894035</v>
+        <v>-38.958274026068253</v>
       </c>
       <c r="C26" s="0">
-        <v>16.437687695214116</v>
+        <v>16.416454560567544</v>
       </c>
       <c r="D26" s="0">
-        <v>7.1239589413185698</v>
+        <v>7.1519139611667963</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="B27" s="0">
-        <v>28.811557578242127</v>
+        <v>28.856087485849759</v>
       </c>
       <c r="C27" s="0">
-        <v>20.128518785164644</v>
+        <v>20.164263973099484</v>
       </c>
       <c r="D27" s="0">
-        <v>30.95596551399386</v>
+        <v>30.651281284445307</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="B28" s="0">
-        <v>17.723057348900163</v>
+        <v>17.610305593874497</v>
       </c>
       <c r="C28" s="0">
-        <v>26.131648376208055</v>
+        <v>26.129182443438207</v>
       </c>
       <c r="D28" s="0">
-        <v>31.110671718565246</v>
+        <v>31.047711813984741</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="B29" s="0">
-        <v>9.9105013240325057</v>
+        <v>9.9077978452714408</v>
       </c>
       <c r="C29" s="0">
-        <v>25.796974885707133</v>
+        <v>25.868034504238139</v>
       </c>
       <c r="D29" s="0">
-        <v>28.726743311227573</v>
+        <v>28.684693368088059</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="B30" s="0">
-        <v>-11.488892111621679</v>
+        <v>-11.405942093791385</v>
       </c>
       <c r="C30" s="0">
-        <v>23.377141915772011</v>
+        <v>23.372500680398026</v>
       </c>
       <c r="D30" s="0">
-        <v>14.087025644845074</v>
+        <v>13.90607439441805</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="B31" s="0">
-        <v>-21.322593585811823</v>
+        <v>-20.981413768657315</v>
       </c>
       <c r="C31" s="0">
-        <v>37.433910146710119</v>
+        <v>37.261185910112907</v>
       </c>
       <c r="D31" s="0">
-        <v>16.432632358312194</v>
+        <v>16.597289266642932</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="B32" s="0">
-        <v>-36.241266523300048</v>
+        <v>-36.237703276710242</v>
       </c>
       <c r="C32" s="0">
-        <v>26.471725053618901</v>
+        <v>26.46669746146544</v>
       </c>
       <c r="D32" s="0">
-        <v>13.978228766897997</v>
+        <v>14.081747037571965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>